<commit_message>
Update and tune respiratory diseases.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilator.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\ventilator_scenarios\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDDD072-9DF0-4735-A0BE-B1FAB51F05EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52CC594-223E-46A8-92E5-78C31F675449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26640" yWindow="3030" windowWidth="29880" windowHeight="28455" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24615" yWindow="3030" windowWidth="29880" windowHeight="28455" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Healthy" sheetId="1" r:id="rId1"/>
@@ -782,7 +782,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -821,6 +821,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -848,7 +861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -926,6 +939,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1529,10 +1545,10 @@
       <c r="B13" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="9" t="s">
         <v>60</v>
       </c>
@@ -1895,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686184DF-C2C0-4678-BF86-A08B4E364237}">
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:F52"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2142,10 +2158,10 @@
       <c r="B15" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="9" t="s">
         <v>111</v>
       </c>
@@ -2538,10 +2554,10 @@
       <c r="B33" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="9" t="s">
         <v>113</v>
       </c>
@@ -2551,13 +2567,13 @@
       <c r="A34" s="8">
         <v>2</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
@@ -2934,10 +2950,10 @@
       <c r="B51" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="27"/>
       <c r="G51" s="9" t="s">
         <v>115</v>
       </c>
@@ -2947,13 +2963,13 @@
       <c r="A52" s="8">
         <v>3</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="27"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
@@ -3334,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777CC981-6C3C-48D9-AA91-9BEF926E562A}">
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:F52"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3581,10 +3597,10 @@
       <c r="B15" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="9" t="s">
         <v>140</v>
       </c>
@@ -3594,13 +3610,13 @@
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -3977,10 +3993,10 @@
       <c r="B33" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="9" t="s">
         <v>141</v>
       </c>
@@ -3990,13 +4006,13 @@
       <c r="A34" s="8">
         <v>2</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
@@ -4373,10 +4389,10 @@
       <c r="B51" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="27"/>
       <c r="G51" s="9" t="s">
         <v>142</v>
       </c>
@@ -4386,13 +4402,13 @@
       <c r="A52" s="8">
         <v>3</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="27"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
@@ -5020,10 +5036,10 @@
       <c r="B15" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="9" t="s">
         <v>151</v>
       </c>
@@ -5208,10 +5224,10 @@
       <c r="B24" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="9" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
Respiratory disease calibration based on updated validation targets.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilator.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\ventilator_scenarios\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2735C4-4EE9-4627-806F-DE3003B194ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1018A025-13A2-4847-9E92-F5976A3C1B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23910" yWindow="3030" windowWidth="29880" windowHeight="28455" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27420" yWindow="5955" windowWidth="28245" windowHeight="23445" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Healthy" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="149">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -249,15 +249,6 @@
     <t>range</t>
   </si>
   <si>
-    <t>[9, 10]</t>
-  </si>
-  <si>
-    <t>[9, 12]</t>
-  </si>
-  <si>
-    <t>[45, 55]</t>
-  </si>
-  <si>
     <t>InspiratoryExpiratoryRatio</t>
   </si>
   <si>
@@ -288,18 +279,9 @@
     <t>ShuntFraction</t>
   </si>
   <si>
-    <t>[0.02, 0.05]</t>
-  </si>
-  <si>
     <t>Levitzky2013pulmonary, radermacher2017fifty, petersson2014gas</t>
   </si>
   <si>
-    <t>Levitzky2013pulmonary</t>
-  </si>
-  <si>
-    <t>VD</t>
-  </si>
-  <si>
     <t>RR (set)</t>
   </si>
   <si>
@@ -313,9 +295,6 @@
   </si>
   <si>
     <t>MechanicalVentilatorHealthy</t>
-  </si>
-  <si>
-    <t>AlveolarDeadSpace</t>
   </si>
   <si>
     <t>MechanicalVentilatorARDS</t>
@@ -330,9 +309,6 @@
 }</t>
   </si>
   <si>
-    <t>[41, 45]</t>
-  </si>
-  <si>
     <t>[7.15, 7.34]</t>
   </si>
   <si>
@@ -352,9 +328,6 @@
   </si>
   <si>
     <t>greaterThanValue</t>
-  </si>
-  <si>
-    <t>nuckton2002pulmonary</t>
   </si>
   <si>
     <t>radermacher2017fifty, petersson2014gas</t>
@@ -369,15 +342,6 @@
 }</t>
   </si>
   <si>
-    <t>[11, 13]</t>
-  </si>
-  <si>
-    <t>[13, 16]</t>
-  </si>
-  <si>
-    <t>[31, 40]</t>
-  </si>
-  <si>
     <t>[81, 117]</t>
   </si>
   <si>
@@ -385,15 +349,6 @@
   </si>
   <si>
     <t>[0.959, 0.986]</t>
-  </si>
-  <si>
-    <t>[14, 15]</t>
-  </si>
-  <si>
-    <t>[17, 20]</t>
-  </si>
-  <si>
-    <t>[25, 30]</t>
   </si>
   <si>
     <t>[56, 83]</t>
@@ -508,30 +463,6 @@
     }</t>
   </si>
   <si>
-    <t>[15, 20]</t>
-  </si>
-  <si>
-    <t>[21, 25]</t>
-  </si>
-  <si>
-    <t>[20, 25]</t>
-  </si>
-  <si>
-    <t>[26, 30]</t>
-  </si>
-  <si>
-    <t>[31, 35]</t>
-  </si>
-  <si>
-    <t>[45, 50]</t>
-  </si>
-  <si>
-    <t>[51, 55]</t>
-  </si>
-  <si>
-    <t>[56, 60]</t>
-  </si>
-  <si>
     <t>[7.2, 7.31]</t>
   </si>
   <si>
@@ -714,6 +645,18 @@
           { "Compartment": "RightLung", "Severity": { "Scalar0To1": { "Value": 0.9 }}}]
       }}
     }</t>
+  </si>
+  <si>
+    <t>[0.03, 0.05]</t>
+  </si>
+  <si>
+    <t>PhysiologicDeadSpaceTidalVolumeRatio</t>
+  </si>
+  <si>
+    <t>[0.25, 0.35]</t>
+  </si>
+  <si>
+    <t>VD/VT</t>
   </si>
 </sst>
 </file>
@@ -914,7 +857,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -926,22 +884,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1326,16 +1269,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B14" sqref="B14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="12" customWidth="1"/>
     <col min="4" max="4" width="25" style="12" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="12" customWidth="1"/>
@@ -1347,44 +1290,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="AMG1" s="14"/>
       <c r="AMH1" s="14"/>
       <c r="AMI1" s="14"/>
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="20"/>
+      <c r="A2" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="25"/>
       <c r="E2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="AMG2" s="14"/>
       <c r="AMH2" s="14"/>
       <c r="AMI2" s="14"/>
@@ -1394,13 +1337,13 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1412,11 +1355,11 @@
       <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="3"/>
       <c r="H4" s="16" t="s">
         <v>8</v>
@@ -1435,72 +1378,72 @@
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:1024" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1512,13 +1455,13 @@
       <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
         <v>20</v>
@@ -1528,13 +1471,13 @@
       <c r="A12" s="8">
         <v>1</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
@@ -1542,13 +1485,13 @@
       <c r="A13" s="8">
         <v>1</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="9" t="s">
         <v>60</v>
       </c>
@@ -1558,13 +1501,13 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -1605,13 +1548,13 @@
         <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="E16" s="2">
+        <v>9</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>45</v>
@@ -1629,13 +1572,13 @@
         <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E17" s="2">
+        <v>9</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>46</v>
@@ -1653,13 +1596,13 @@
         <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>29</v>
+      </c>
+      <c r="E18" s="2">
+        <v>55</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>47</v>
@@ -1668,45 +1611,47 @@
     </row>
     <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="2">
-        <v>527</v>
+        <v>62</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="2" t="s">
-        <v>146</v>
+      <c r="G19" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="2">
-        <v>15</v>
-      </c>
-      <c r="F20" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="G20" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H20" s="10"/>
     </row>
@@ -1715,116 +1660,112 @@
         <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="2">
-        <v>0.6</v>
+        <v>527</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E22" s="2">
+        <v>15</v>
+      </c>
+      <c r="F22" s="11"/>
       <c r="G22" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="11"/>
       <c r="G23" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H25" s="10"/>
     </row>
@@ -1833,31 +1774,31 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="2">
-        <v>300</v>
+        <v>62</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>28</v>
@@ -1866,23 +1807,48 @@
         <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="2">
+        <v>300</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="E5:F9"/>
@@ -1891,12 +1857,11 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B10:F10"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1911,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686184DF-C2C0-4678-BF86-A08B4E364237}">
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
@@ -1930,44 +1895,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="AMG1" s="14"/>
       <c r="AMH1" s="14"/>
       <c r="AMI1" s="14"/>
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="20"/>
+      <c r="A2" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="25"/>
       <c r="E2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+        <v>77</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="AMG2" s="14"/>
       <c r="AMH2" s="14"/>
       <c r="AMI2" s="14"/>
@@ -1977,13 +1942,13 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1995,11 +1960,11 @@
       <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="3"/>
       <c r="H4" s="16" t="s">
         <v>8</v>
@@ -2018,72 +1983,72 @@
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:1024" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2095,13 +2060,13 @@
       <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
@@ -2109,15 +2074,15 @@
       <c r="A12" s="8">
         <v>1</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="B12" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H12" s="9"/>
     </row>
@@ -2125,13 +2090,13 @@
       <c r="A13" s="8">
         <v>1</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
         <v>20</v>
@@ -2141,13 +2106,13 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -2155,29 +2120,29 @@
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="B15" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="9" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -2218,13 +2183,13 @@
         <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>45</v>
@@ -2242,13 +2207,13 @@
         <v>39</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>46</v>
@@ -2266,13 +2231,13 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>88</v>
+        <v>29</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>47</v>
@@ -2281,45 +2246,47 @@
     </row>
     <row r="21" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="2">
-        <v>452</v>
+        <v>0.3</v>
       </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="2" t="s">
-        <v>146</v>
+      <c r="G21" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="2">
-        <v>17</v>
-      </c>
-      <c r="F22" s="11"/>
+        <v>0.15</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="G22" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H22" s="10"/>
     </row>
@@ -2328,116 +2295,112 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="2">
-        <v>0.9</v>
+        <v>452</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E24" s="2">
+        <v>17</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F25" s="11"/>
       <c r="G25" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H27" s="10"/>
     </row>
@@ -2446,22 +2409,22 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H28" s="10"/>
     </row>
@@ -2470,22 +2433,22 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0.1</v>
+        <v>62</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H29" s="10"/>
     </row>
@@ -2494,22 +2457,22 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="G30" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H30" s="10"/>
     </row>
@@ -2517,13 +2480,13 @@
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="1" t="s">
         <v>6</v>
       </c>
@@ -2535,15 +2498,15 @@
       <c r="A32" s="8">
         <v>2</v>
       </c>
-      <c r="B32" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
+      <c r="B32" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="9" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="H32" s="9"/>
     </row>
@@ -2551,15 +2514,15 @@
       <c r="A33" s="8">
         <v>2</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="27"/>
+      <c r="B33" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="9" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="H33" s="9"/>
     </row>
@@ -2567,13 +2530,13 @@
       <c r="A34" s="8">
         <v>2</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="27"/>
+      <c r="B34" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
@@ -2614,13 +2577,13 @@
         <v>39</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>99</v>
+        <v>29</v>
+      </c>
+      <c r="E36" s="2">
+        <v>10</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>45</v>
@@ -2638,13 +2601,13 @@
         <v>39</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>100</v>
+        <v>29</v>
+      </c>
+      <c r="E37" s="2">
+        <v>10</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>46</v>
@@ -2662,13 +2625,13 @@
         <v>38</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>101</v>
+        <v>29</v>
+      </c>
+      <c r="E38" s="2">
+        <v>35</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>47</v>
@@ -2677,45 +2640,47 @@
     </row>
     <row r="39" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E39" s="2">
-        <v>452</v>
+        <v>0.45</v>
       </c>
       <c r="F39" s="11"/>
-      <c r="G39" s="2" t="s">
-        <v>146</v>
+      <c r="G39" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="2">
-        <v>20</v>
-      </c>
-      <c r="F40" s="11"/>
+        <v>0.4</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="G40" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H40" s="10"/>
     </row>
@@ -2724,116 +2689,112 @@
         <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E41" s="2">
-        <v>0.9</v>
+        <v>452</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E42" s="2">
+        <v>20</v>
+      </c>
+      <c r="F42" s="11"/>
       <c r="G42" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F43" s="11"/>
       <c r="G43" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H45" s="10"/>
     </row>
@@ -2842,22 +2803,22 @@
         <v>26</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H46" s="10"/>
     </row>
@@ -2866,22 +2827,22 @@
         <v>26</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E47" s="2">
-        <v>0.2</v>
+        <v>62</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H47" s="10"/>
     </row>
@@ -2890,22 +2851,22 @@
         <v>26</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H48" s="10"/>
     </row>
@@ -2913,13 +2874,13 @@
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
       <c r="G49" s="1" t="s">
         <v>6</v>
       </c>
@@ -2931,15 +2892,15 @@
       <c r="A50" s="8">
         <v>3</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
       <c r="G50" s="9" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="H50" s="9"/>
     </row>
@@ -2947,15 +2908,15 @@
       <c r="A51" s="8">
         <v>3</v>
       </c>
-      <c r="B51" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="27"/>
+      <c r="B51" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="H51" s="9"/>
     </row>
@@ -2963,13 +2924,13 @@
       <c r="A52" s="8">
         <v>3</v>
       </c>
-      <c r="B52" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="27"/>
+      <c r="B52" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
@@ -3010,13 +2971,13 @@
         <v>39</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>105</v>
+        <v>29</v>
+      </c>
+      <c r="E54" s="2">
+        <v>12</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>45</v>
@@ -3034,13 +2995,13 @@
         <v>39</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>106</v>
+        <v>29</v>
+      </c>
+      <c r="E55" s="2">
+        <v>12</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>46</v>
@@ -3058,13 +3019,13 @@
         <v>38</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>107</v>
+        <v>29</v>
+      </c>
+      <c r="E56" s="2">
+        <v>25</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>47</v>
@@ -3073,45 +3034,47 @@
     </row>
     <row r="57" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E57" s="2">
-        <v>452</v>
+        <v>0.65</v>
       </c>
       <c r="F57" s="11"/>
-      <c r="G57" s="2" t="s">
-        <v>146</v>
+      <c r="G57" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E58" s="2">
-        <v>25</v>
-      </c>
-      <c r="F58" s="11"/>
+        <v>0.7</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="G58" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H58" s="10"/>
     </row>
@@ -3120,116 +3083,112 @@
         <v>37</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E59" s="2">
-        <v>0.9</v>
+        <v>452</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E60" s="2">
+        <v>25</v>
+      </c>
+      <c r="F60" s="11"/>
       <c r="G60" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F61" s="11"/>
       <c r="G61" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G63" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H63" s="10"/>
     </row>
@@ -3238,22 +3197,22 @@
         <v>26</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64" s="2">
-        <v>100</v>
+        <v>62</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H64" s="10"/>
     </row>
@@ -3262,22 +3221,22 @@
         <v>26</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E65" s="2">
-        <v>0.4</v>
+        <v>62</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H65" s="10"/>
     </row>
@@ -3286,32 +3245,41 @@
         <v>26</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" s="2">
+        <v>100</v>
+      </c>
+      <c r="F66" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="2">
-        <v>2</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="G66" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H66" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
@@ -3322,20 +3290,11 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -3369,44 +3328,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="AMG1" s="14"/>
       <c r="AMH1" s="14"/>
       <c r="AMI1" s="14"/>
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="20"/>
+      <c r="A2" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="25"/>
       <c r="E2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+        <v>77</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="AMG2" s="14"/>
       <c r="AMH2" s="14"/>
       <c r="AMI2" s="14"/>
@@ -3416,13 +3375,13 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
@@ -3434,11 +3393,11 @@
       <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="3"/>
       <c r="H4" s="16" t="s">
         <v>8</v>
@@ -3457,72 +3416,72 @@
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:1024" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3534,13 +3493,13 @@
       <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
@@ -3548,15 +3507,15 @@
       <c r="A12" s="8">
         <v>1</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="9" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="H12" s="9"/>
     </row>
@@ -3564,13 +3523,13 @@
       <c r="A13" s="8">
         <v>1</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
         <v>20</v>
@@ -3580,13 +3539,13 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -3594,15 +3553,15 @@
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="B15" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="9" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="H15" s="9"/>
     </row>
@@ -3610,13 +3569,13 @@
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
+      <c r="B16" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -3657,13 +3616,13 @@
         <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>126</v>
+        <v>29</v>
+      </c>
+      <c r="E18" s="2">
+        <v>10</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>45</v>
@@ -3681,13 +3640,13 @@
         <v>39</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>128</v>
+        <v>29</v>
+      </c>
+      <c r="E19" s="2">
+        <v>10</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>46</v>
@@ -3705,13 +3664,13 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>131</v>
+        <v>29</v>
+      </c>
+      <c r="E20" s="2">
+        <v>60</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>47</v>
@@ -3720,45 +3679,47 @@
     </row>
     <row r="21" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="2">
-        <v>678</v>
+        <v>0.35</v>
       </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="2" t="s">
-        <v>146</v>
+      <c r="G21" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="2">
-        <v>12</v>
-      </c>
-      <c r="F22" s="11"/>
+        <v>0.15</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="G22" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H22" s="10"/>
     </row>
@@ -3767,116 +3728,112 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="2">
-        <v>0.43</v>
+        <v>678</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E24" s="2">
+        <v>12</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F25" s="11"/>
       <c r="G25" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H27" s="10"/>
     </row>
@@ -3885,22 +3842,22 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H28" s="10"/>
     </row>
@@ -3909,22 +3866,22 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H29" s="10"/>
     </row>
@@ -3933,22 +3890,22 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="G30" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H30" s="10"/>
     </row>
@@ -3956,13 +3913,13 @@
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="1" t="s">
         <v>6</v>
       </c>
@@ -3974,15 +3931,15 @@
       <c r="A32" s="8">
         <v>2</v>
       </c>
-      <c r="B32" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
+      <c r="B32" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="9" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="H32" s="9"/>
     </row>
@@ -3990,15 +3947,15 @@
       <c r="A33" s="8">
         <v>2</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="27"/>
+      <c r="B33" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="9" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="H33" s="9"/>
     </row>
@@ -4006,13 +3963,13 @@
       <c r="A34" s="8">
         <v>2</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="27"/>
+      <c r="B34" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
@@ -4053,13 +4010,13 @@
         <v>39</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>127</v>
+        <v>29</v>
+      </c>
+      <c r="E36" s="2">
+        <v>15</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>45</v>
@@ -4077,13 +4034,13 @@
         <v>39</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>129</v>
+        <v>29</v>
+      </c>
+      <c r="E37" s="2">
+        <v>25</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>46</v>
@@ -4101,13 +4058,13 @@
         <v>38</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>132</v>
+        <v>29</v>
+      </c>
+      <c r="E38" s="2">
+        <v>68</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>47</v>
@@ -4116,45 +4073,47 @@
     </row>
     <row r="39" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E39" s="2">
-        <v>640</v>
+        <v>0.5</v>
       </c>
       <c r="F39" s="11"/>
-      <c r="G39" s="2" t="s">
-        <v>146</v>
+      <c r="G39" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="2">
-        <v>14</v>
-      </c>
-      <c r="F40" s="11"/>
+        <v>0.25</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="G40" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H40" s="10"/>
     </row>
@@ -4163,116 +4122,112 @@
         <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E41" s="2">
-        <v>0.43</v>
+        <v>640</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E42" s="2">
+        <v>14</v>
+      </c>
+      <c r="F42" s="11"/>
       <c r="G42" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F43" s="11"/>
       <c r="G43" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H45" s="10"/>
     </row>
@@ -4281,22 +4236,22 @@
         <v>26</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H46" s="10"/>
     </row>
@@ -4305,22 +4260,22 @@
         <v>26</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H47" s="10"/>
     </row>
@@ -4329,22 +4284,22 @@
         <v>26</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H48" s="10"/>
     </row>
@@ -4352,13 +4307,13 @@
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
       <c r="G49" s="1" t="s">
         <v>6</v>
       </c>
@@ -4370,15 +4325,15 @@
       <c r="A50" s="8">
         <v>3</v>
       </c>
-      <c r="B50" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
+      <c r="B50" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
       <c r="G50" s="9" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="H50" s="9"/>
     </row>
@@ -4386,15 +4341,15 @@
       <c r="A51" s="8">
         <v>3</v>
       </c>
-      <c r="B51" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="27"/>
+      <c r="B51" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="9" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="H51" s="9"/>
     </row>
@@ -4402,13 +4357,13 @@
       <c r="A52" s="8">
         <v>3</v>
       </c>
-      <c r="B52" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="27"/>
+      <c r="B52" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
@@ -4449,13 +4404,13 @@
         <v>39</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>107</v>
+        <v>29</v>
+      </c>
+      <c r="E54" s="2">
+        <v>20</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>45</v>
@@ -4473,13 +4428,13 @@
         <v>39</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>130</v>
+        <v>29</v>
+      </c>
+      <c r="E55" s="2">
+        <v>40</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>46</v>
@@ -4497,13 +4452,13 @@
         <v>38</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>133</v>
+        <v>29</v>
+      </c>
+      <c r="E56" s="2">
+        <v>75</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>47</v>
@@ -4512,45 +4467,47 @@
     </row>
     <row r="57" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E57" s="2">
-        <v>678</v>
+        <v>0.7</v>
       </c>
       <c r="F57" s="11"/>
-      <c r="G57" s="2" t="s">
-        <v>146</v>
+      <c r="G57" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E58" s="2">
-        <v>15</v>
-      </c>
-      <c r="F58" s="11"/>
+        <v>0.4</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="G58" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H58" s="10"/>
     </row>
@@ -4559,116 +4516,112 @@
         <v>37</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E59" s="2">
-        <v>0.43</v>
+        <v>678</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E60" s="2">
+        <v>15</v>
+      </c>
+      <c r="F60" s="11"/>
       <c r="G60" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F61" s="11"/>
       <c r="G61" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G63" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H63" s="10"/>
     </row>
@@ -4677,22 +4630,22 @@
         <v>26</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H64" s="10"/>
     </row>
@@ -4701,22 +4654,22 @@
         <v>26</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E65" s="2">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="H65" s="10"/>
     </row>
@@ -4725,27 +4678,47 @@
         <v>26</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F66" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="2">
-        <v>2</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="G66" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H66" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B51:F51"/>
     <mergeCell ref="B52:F52"/>
@@ -4755,26 +4728,6 @@
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -4790,7 +4743,7 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4808,44 +4761,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="AMG1" s="14"/>
       <c r="AMH1" s="14"/>
       <c r="AMI1" s="14"/>
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="20"/>
+      <c r="A2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="25"/>
       <c r="E2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+        <v>77</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="AMG2" s="14"/>
       <c r="AMH2" s="14"/>
       <c r="AMI2" s="14"/>
@@ -4855,13 +4808,13 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
@@ -4873,11 +4826,11 @@
       <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="3"/>
       <c r="H4" s="16" t="s">
         <v>8</v>
@@ -4896,72 +4849,72 @@
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:1024" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4973,13 +4926,13 @@
       <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
@@ -4987,15 +4940,15 @@
       <c r="A12" s="8">
         <v>1</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="B12" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="9" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="H12" s="9"/>
     </row>
@@ -5003,13 +4956,13 @@
       <c r="A13" s="8">
         <v>1</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
         <v>20</v>
@@ -5019,13 +4972,13 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -5033,15 +4986,15 @@
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="B15" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="9" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="H15" s="9"/>
     </row>
@@ -5049,13 +5002,13 @@
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -5103,7 +5056,7 @@
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="2" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="H18" s="10"/>
     </row>
@@ -5125,7 +5078,7 @@
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H19" s="10"/>
     </row>
@@ -5134,7 +5087,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>28</v>
@@ -5147,7 +5100,7 @@
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H20" s="10"/>
     </row>
@@ -5165,13 +5118,13 @@
         <v>62</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="H21" s="10"/>
     </row>
@@ -5180,7 +5133,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -5189,13 +5142,13 @@
         <v>62</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="H22" s="10"/>
     </row>
@@ -5203,13 +5156,13 @@
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="1" t="s">
         <v>6</v>
       </c>
@@ -5221,15 +5174,15 @@
       <c r="A24" s="8">
         <v>2</v>
       </c>
-      <c r="B24" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="27"/>
+      <c r="B24" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="9" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="H24" s="9"/>
     </row>
@@ -5237,13 +5190,13 @@
       <c r="A25" s="8">
         <v>2</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="B25" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
     </row>
@@ -5291,7 +5244,7 @@
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="2" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="H27" s="10"/>
     </row>
@@ -5313,7 +5266,7 @@
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H28" s="10"/>
     </row>
@@ -5322,7 +5275,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>28</v>
@@ -5335,7 +5288,7 @@
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H29" s="10"/>
     </row>
@@ -5350,13 +5303,13 @@
         <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E30" s="2">
         <v>1</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>50</v>
@@ -5380,7 +5333,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>51</v>
@@ -5401,13 +5354,13 @@
         <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="H32" s="10"/>
     </row>
@@ -5428,10 +5381,10 @@
         <v>1</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="H33" s="10"/>
     </row>
@@ -5440,7 +5393,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>28</v>
@@ -5449,13 +5402,13 @@
         <v>62</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="H34" s="10"/>
     </row>
@@ -5464,7 +5417,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>28</v>
@@ -5476,15 +5429,29 @@
         <v>1</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="H35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B24:F24"/>
@@ -5495,20 +5462,6 @@
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>